<commit_message>
Update GHG source / plastics source / requirements.
</commit_message>
<xml_diff>
--- a/Data/Concordances/openIO_IW_concordance.xlsx
+++ b/Data/Concordances/openIO_IW_concordance.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\OpenIOCanada\Data\Concordances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A7D7F3-B398-474D-A6EA-0DE5AD94A9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3574FB-69EC-4468-A36E-33486E50E532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,9 @@
     <sheet name="2019" sheetId="4" r:id="rId4"/>
     <sheet name="2020" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2019'!$A$1:$B$359</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1291,9 +1294,6 @@
     <t>Beryllium</t>
   </si>
   <si>
-    <t>Berrylium</t>
-  </si>
-  <si>
     <t>Bismuth</t>
   </si>
   <si>
@@ -1850,6 +1850,9 @@
   </si>
   <si>
     <t>Butane, perfluorocyclo-, PFC-318</t>
+  </si>
+  <si>
+    <t>Berylium</t>
   </si>
 </sst>
 </file>
@@ -2205,7 +2208,7 @@
   <dimension ref="A1:B399"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B25"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2248,170 +2251,170 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -2457,7 +2460,7 @@
         <v>418</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -2465,23 +2468,23 @@
         <v>419</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>420</v>
+        <v>606</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -2518,111 +2521,111 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B39" s="4"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="B45" s="4" t="s">
         <v>429</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B47" s="4"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B49" s="4"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B50" s="4"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="B52" s="4" t="s">
         <v>434</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B53" s="4"/>
     </row>
@@ -2636,18 +2639,18 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -2668,16 +2671,16 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B59" s="4"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -2690,107 +2693,107 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B63" s="4"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="B66" s="4" t="s">
         <v>442</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B68" s="4"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B69" s="4"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="B71" s="4" t="s">
         <v>446</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B72" s="4"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B74" s="4"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B75" s="4"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B76" s="4"/>
     </row>
@@ -2812,64 +2815,64 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B85" s="4"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
@@ -2882,15 +2885,15 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B89" s="4"/>
     </row>
@@ -2904,10 +2907,10 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
@@ -2950,10 +2953,10 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="B97" s="3" t="s">
         <v>499</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
@@ -3068,7 +3071,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B112" s="3"/>
     </row>
@@ -3114,7 +3117,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>263</v>
@@ -3154,7 +3157,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B123" s="3"/>
     </row>
@@ -3238,7 +3241,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>117</v>
@@ -3262,7 +3265,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B137" s="3"/>
     </row>
@@ -3276,7 +3279,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B139" s="3"/>
     </row>
@@ -3330,7 +3333,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B146" s="3"/>
     </row>
@@ -3350,13 +3353,13 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B149" s="3"/>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B150" s="3"/>
     </row>
@@ -3604,31 +3607,31 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B183" s="3"/>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B184" s="3"/>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B185" s="3"/>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B186" s="3"/>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B187" s="3"/>
     </row>
@@ -3666,15 +3669,15 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="B192" s="3" t="s">
         <v>515</v>
-      </c>
-      <c r="B192" s="3" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B193" s="3"/>
     </row>
@@ -3710,7 +3713,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" s="4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B198" s="3" t="s">
         <v>288</v>
@@ -3758,10 +3761,10 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="B204" s="3" t="s">
         <v>519</v>
-      </c>
-      <c r="B204" s="3" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
@@ -3830,10 +3833,10 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="B213" s="3" t="s">
         <v>521</v>
-      </c>
-      <c r="B213" s="3" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
@@ -3846,19 +3849,19 @@
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B215" s="3"/>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B216" s="3"/>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B217" s="3"/>
     </row>
@@ -3886,7 +3889,7 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" s="4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B221" s="3" t="s">
         <v>304</v>
@@ -3934,19 +3937,19 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B228" s="3"/>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" s="4" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B229" s="3"/>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" s="4" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B230" s="3" t="s">
         <v>187</v>
@@ -3992,7 +3995,7 @@
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" s="4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B236" s="3"/>
     </row>
@@ -4088,7 +4091,7 @@
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249" s="4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B249" s="3" t="s">
         <v>392</v>
@@ -4128,7 +4131,7 @@
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B254" s="3"/>
     </row>
@@ -4188,19 +4191,19 @@
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A262" s="4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B262" s="3"/>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A263" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B263" s="3"/>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A264" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B264" s="3"/>
     </row>
@@ -4209,7 +4212,7 @@
         <v>235</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.3">
@@ -4282,13 +4285,13 @@
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A275" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B275" s="3"/>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A276" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B276" s="3"/>
     </row>
@@ -4354,13 +4357,13 @@
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A285" s="4" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B285" s="3"/>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A286" s="4" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B286" s="3"/>
     </row>
@@ -4398,7 +4401,7 @@
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A291" s="4" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B291" s="3"/>
     </row>
@@ -4420,7 +4423,7 @@
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A294" s="4" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B294" s="3" t="s">
         <v>53</v>
@@ -4428,7 +4431,7 @@
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A295" s="4" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B295" s="3"/>
     </row>
@@ -4442,19 +4445,19 @@
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A297" s="4" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B297" s="3"/>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A298" s="4" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B298" s="3"/>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A299" s="4" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B299" s="3" t="s">
         <v>109</v>
@@ -4462,25 +4465,25 @@
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A300" s="4" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B300" s="3"/>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A301" s="4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B301" s="3"/>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A302" s="4" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B302" s="3"/>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A303" s="4" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B303" s="3"/>
     </row>
@@ -4500,21 +4503,21 @@
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A306" s="4" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A307" s="4" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B307" s="3"/>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A308" s="4" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B308" s="3"/>
     </row>
@@ -4528,13 +4531,13 @@
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A310" s="4" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B310" s="3"/>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A311" s="4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B311" s="3" t="s">
         <v>288</v>
@@ -4558,18 +4561,18 @@
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A314" s="4" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A315" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B315" s="3" t="s">
         <v>557</v>
-      </c>
-      <c r="B315" s="3" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.3">
@@ -4602,19 +4605,19 @@
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A320" s="4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B320" s="3"/>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A321" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B321" s="3"/>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A322" s="4" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B322" s="3" t="s">
         <v>304</v>
@@ -4672,7 +4675,7 @@
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A330" s="4" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B330" s="3"/>
     </row>
@@ -4696,13 +4699,13 @@
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A334" s="4" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B334" s="3"/>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A335" s="4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B335" s="3"/>
     </row>
@@ -4720,7 +4723,7 @@
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A338" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B338" s="3"/>
     </row>
@@ -4742,13 +4745,13 @@
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A341" s="4" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B341" s="3"/>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A342" s="4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B342" s="3"/>
     </row>
@@ -4780,7 +4783,7 @@
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A347" s="4" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B347" s="3"/>
     </row>
@@ -4802,7 +4805,7 @@
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A350" s="4" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B350" s="3" t="s">
         <v>341</v>
@@ -4810,7 +4813,7 @@
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A351" s="4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B351" s="3"/>
     </row>
@@ -4864,7 +4867,7 @@
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A359" s="4" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B359" s="3" t="s">
         <v>274</v>
@@ -4888,7 +4891,7 @@
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A362" s="4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B362" s="3"/>
     </row>
@@ -4934,7 +4937,7 @@
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A368" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B368" s="3" t="s">
         <v>337</v>
@@ -5024,7 +5027,7 @@
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A380" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B380" s="3" t="s">
         <v>341</v>
@@ -5056,7 +5059,7 @@
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A384" s="4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B384" s="3" t="s">
         <v>385</v>
@@ -5064,7 +5067,7 @@
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A385" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B385" s="3"/>
     </row>
@@ -5094,7 +5097,7 @@
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A389" s="4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B389" s="3" t="s">
         <v>274</v>
@@ -5150,10 +5153,10 @@
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A396" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.3">
@@ -5189,8 +5192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF3D242-5B0E-417F-BDFF-9399A3C06D58}">
   <dimension ref="A1:B401"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5233,170 +5236,170 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -5442,7 +5445,7 @@
         <v>418</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -5450,23 +5453,23 @@
         <v>419</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>420</v>
+        <v>606</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -5503,111 +5506,111 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B39" s="4"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="B45" s="4" t="s">
         <v>429</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B47" s="4"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B49" s="4"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B50" s="4"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="B52" s="4" t="s">
         <v>434</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B53" s="4"/>
     </row>
@@ -5621,18 +5624,18 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -5653,16 +5656,16 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B59" s="4"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -5675,107 +5678,107 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B63" s="4"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="B66" s="4" t="s">
         <v>442</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B68" s="4"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B69" s="4"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="B71" s="4" t="s">
         <v>446</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B72" s="4"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B74" s="4"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B75" s="4"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B76" s="4"/>
     </row>
@@ -5797,64 +5800,64 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B85" s="4"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
@@ -5867,15 +5870,15 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B89" s="4"/>
     </row>
@@ -5889,10 +5892,10 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
@@ -5935,10 +5938,10 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="B97" s="3" t="s">
         <v>499</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
@@ -5975,7 +5978,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B102" s="3"/>
     </row>
@@ -6013,10 +6016,10 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
@@ -6067,7 +6070,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B114" s="3"/>
     </row>
@@ -6113,7 +6116,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>263</v>
@@ -6153,7 +6156,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B125" s="3"/>
     </row>
@@ -6243,7 +6246,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>117</v>
@@ -6267,7 +6270,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B140" s="3"/>
     </row>
@@ -6281,7 +6284,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B142" s="3"/>
     </row>
@@ -6349,13 +6352,13 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B151" s="3"/>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B152" s="3"/>
     </row>
@@ -6603,31 +6606,31 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B185" s="3"/>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B186" s="3"/>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B187" s="3"/>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B188" s="3"/>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B189" s="3"/>
     </row>
@@ -6665,15 +6668,15 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="B194" s="3" t="s">
         <v>515</v>
-      </c>
-      <c r="B194" s="3" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B195" s="3"/>
     </row>
@@ -6717,7 +6720,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" s="4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B201" s="3" t="s">
         <v>288</v>
@@ -6765,10 +6768,10 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="B207" s="3" t="s">
         <v>519</v>
-      </c>
-      <c r="B207" s="3" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
@@ -6845,19 +6848,19 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B217" s="3"/>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B218" s="3"/>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B219" s="3"/>
     </row>
@@ -6885,7 +6888,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" s="4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B223" s="3" t="s">
         <v>304</v>
@@ -6933,19 +6936,19 @@
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B230" s="3"/>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" s="4" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B231" s="3"/>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" s="4" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B232" s="3" t="s">
         <v>187</v>
@@ -6991,7 +6994,7 @@
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238" s="4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B238" s="3"/>
     </row>
@@ -7087,7 +7090,7 @@
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251" s="4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B251" s="3" t="s">
         <v>392</v>
@@ -7127,7 +7130,7 @@
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B256" s="3"/>
     </row>
@@ -7187,19 +7190,19 @@
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A264" s="4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B264" s="3"/>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A265" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B265" s="3"/>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A266" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B266" s="3"/>
     </row>
@@ -7208,7 +7211,7 @@
         <v>235</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.3">
@@ -7281,13 +7284,13 @@
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A277" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B277" s="3"/>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A278" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B278" s="3"/>
     </row>
@@ -7353,13 +7356,13 @@
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A287" s="4" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B287" s="3"/>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A288" s="4" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B288" s="3"/>
     </row>
@@ -7397,7 +7400,7 @@
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A293" s="4" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B293" s="3"/>
     </row>
@@ -7419,7 +7422,7 @@
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A296" s="4" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B296" s="3" t="s">
         <v>53</v>
@@ -7427,7 +7430,7 @@
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A297" s="4" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B297" s="3"/>
     </row>
@@ -7441,19 +7444,19 @@
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A299" s="4" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B299" s="3"/>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A300" s="4" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B300" s="3"/>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A301" s="4" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B301" s="3" t="s">
         <v>109</v>
@@ -7461,25 +7464,25 @@
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A302" s="4" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B302" s="3"/>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A303" s="4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B303" s="3"/>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A304" s="4" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B304" s="3"/>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A305" s="4" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B305" s="3"/>
     </row>
@@ -7499,21 +7502,21 @@
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A308" s="4" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A309" s="4" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B309" s="3"/>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A310" s="4" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B310" s="3"/>
     </row>
@@ -7527,13 +7530,13 @@
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A312" s="4" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B312" s="3"/>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A313" s="4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B313" s="3" t="s">
         <v>288</v>
@@ -7557,18 +7560,18 @@
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A316" s="4" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A317" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B317" s="3" t="s">
         <v>557</v>
-      </c>
-      <c r="B317" s="3" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.3">
@@ -7601,19 +7604,19 @@
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A322" s="4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B322" s="3"/>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A323" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B323" s="3"/>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A324" s="4" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B324" s="3" t="s">
         <v>304</v>
@@ -7671,7 +7674,7 @@
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A332" s="4" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B332" s="3"/>
     </row>
@@ -7695,13 +7698,13 @@
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A336" s="4" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B336" s="3"/>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A337" s="4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B337" s="3"/>
     </row>
@@ -7719,7 +7722,7 @@
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A340" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B340" s="3"/>
     </row>
@@ -7741,13 +7744,13 @@
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A343" s="4" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B343" s="3"/>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A344" s="4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B344" s="3"/>
     </row>
@@ -7779,7 +7782,7 @@
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A349" s="4" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B349" s="3"/>
     </row>
@@ -7801,7 +7804,7 @@
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A352" s="4" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B352" s="3" t="s">
         <v>341</v>
@@ -7809,7 +7812,7 @@
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A353" s="4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B353" s="3"/>
     </row>
@@ -7863,7 +7866,7 @@
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A361" s="4" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B361" s="3" t="s">
         <v>274</v>
@@ -7887,7 +7890,7 @@
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A364" s="4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B364" s="3"/>
     </row>
@@ -7933,7 +7936,7 @@
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A370" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B370" s="3" t="s">
         <v>337</v>
@@ -8023,7 +8026,7 @@
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A382" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B382" s="3" t="s">
         <v>341</v>
@@ -8055,7 +8058,7 @@
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A386" s="4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B386" s="3" t="s">
         <v>385</v>
@@ -8063,7 +8066,7 @@
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A387" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B387" s="3"/>
     </row>
@@ -8093,7 +8096,7 @@
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A391" s="4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B391" s="3" t="s">
         <v>274</v>
@@ -8149,10 +8152,10 @@
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A398" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.3">
@@ -8188,8 +8191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B362"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8232,162 +8235,162 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -8433,7 +8436,7 @@
         <v>418</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -8441,23 +8444,23 @@
         <v>419</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>420</v>
+        <v>606</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -8494,111 +8497,111 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B38" s="4"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>429</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B46" s="4"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B48" s="4"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B49" s="4"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>434</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B52" s="4"/>
     </row>
@@ -8612,18 +8615,18 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -8644,16 +8647,16 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B58" s="4"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -8666,107 +8669,107 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B62" s="4"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="B65" s="4" t="s">
         <v>442</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B67" s="4"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B68" s="4"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="B70" s="4" t="s">
         <v>446</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B71" s="4"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B73" s="4"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B74" s="4"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B75" s="4"/>
     </row>
@@ -8788,64 +8791,64 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B84" s="4"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
@@ -8858,15 +8861,15 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B88" s="4"/>
     </row>
@@ -8880,10 +8883,10 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
@@ -10954,8 +10957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A058F9-6758-4D54-A3D6-4FA2C9A64680}">
   <dimension ref="A1:B359"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10998,162 +11001,162 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -11199,7 +11202,7 @@
         <v>418</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -11207,23 +11210,23 @@
         <v>419</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>420</v>
+        <v>606</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -11260,111 +11263,111 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B38" s="4"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>429</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B46" s="4"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B48" s="4"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B49" s="4"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>434</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B52" s="4"/>
     </row>
@@ -11378,18 +11381,18 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -11410,16 +11413,16 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B58" s="4"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -11432,107 +11435,107 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B62" s="4"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="B65" s="4" t="s">
         <v>442</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B67" s="4"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B68" s="4"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="B70" s="4" t="s">
         <v>446</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B71" s="4"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B73" s="4"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B74" s="4"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B75" s="4"/>
     </row>
@@ -11554,64 +11557,64 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B84" s="4"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
@@ -11624,15 +11627,15 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B88" s="4"/>
     </row>
@@ -11646,10 +11649,10 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
@@ -12157,7 +12160,7 @@
         <v>104</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
@@ -13689,6 +13692,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B359" xr:uid="{55A058F9-6758-4D54-A3D6-4FA2C9A64680}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -13697,8 +13701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B22D727-350A-4A8A-A4D0-F1E062323C6C}">
   <dimension ref="A1:B352"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13741,162 +13745,162 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -13942,7 +13946,7 @@
         <v>418</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -13950,23 +13954,23 @@
         <v>419</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>420</v>
+        <v>606</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -14003,111 +14007,111 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B38" s="4"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>429</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B46" s="4"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B48" s="4"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B49" s="4"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>434</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B52" s="4"/>
     </row>
@@ -14121,18 +14125,18 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -14153,16 +14157,16 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B58" s="4"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -14175,107 +14179,107 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B62" s="4"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="B65" s="4" t="s">
         <v>442</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B67" s="4"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B68" s="4"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="B70" s="4" t="s">
         <v>446</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B71" s="4"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B73" s="4"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B74" s="4"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B75" s="4"/>
     </row>
@@ -14297,64 +14301,64 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B84" s="4"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
@@ -14367,15 +14371,15 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B88" s="4"/>
     </row>
@@ -14389,10 +14393,10 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
@@ -14451,10 +14455,10 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="B98" s="3" t="s">
         <v>581</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
@@ -14507,10 +14511,10 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="B105" s="3" t="s">
         <v>583</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
@@ -14897,13 +14901,13 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B156" s="3"/>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B157" s="3"/>
     </row>
@@ -15437,10 +15441,10 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="B229" s="3" t="s">
         <v>588</v>
-      </c>
-      <c r="B229" s="3" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
@@ -15453,7 +15457,7 @@
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" s="3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B231" s="3"/>
     </row>

</xml_diff>